<commit_message>
sorting updated, chart added
</commit_message>
<xml_diff>
--- a/etc/perfromances/PerformanceTests.xlsx
+++ b/etc/perfromances/PerformanceTests.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="24735" windowHeight="12360" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="24735" windowHeight="12360" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BeanUtil" sheetId="1" r:id="rId1"/>
     <sheet name="Proxetta" sheetId="2" r:id="rId2"/>
     <sheet name="JDateTime" sheetId="3" r:id="rId3"/>
+    <sheet name="Sorting" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>test #1</t>
   </si>
@@ -37,6 +38,15 @@
   </si>
   <si>
     <t>calendar</t>
+  </si>
+  <si>
+    <t>jodd merge</t>
+  </si>
+  <si>
+    <t>jodd quick</t>
+  </si>
+  <si>
+    <t>java</t>
   </si>
 </sst>
 </file>
@@ -209,25 +219,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="62757504"/>
-        <c:axId val="62767488"/>
+        <c:axId val="60926976"/>
+        <c:axId val="60936960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="62757504"/>
+        <c:axId val="60926976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62767488"/>
+        <c:crossAx val="60936960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62767488"/>
+        <c:axId val="60936960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -255,7 +265,7 @@
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62757504"/>
+        <c:crossAx val="60926976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="20"/>
@@ -280,8 +290,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.79650338228269402"/>
-          <c:y val="0.15320456256640846"/>
+          <c:x val="0.79650338228269391"/>
+          <c:y val="0.15320456256640849"/>
           <c:w val="0.17479472600171553"/>
           <c:h val="0.14658476001491769"/>
         </c:manualLayout>
@@ -301,7 +311,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -413,25 +423,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="62830848"/>
-        <c:axId val="62873600"/>
+        <c:axId val="61012608"/>
+        <c:axId val="61108608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="62830848"/>
+        <c:axId val="61012608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62873600"/>
+        <c:crossAx val="61108608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62873600"/>
+        <c:axId val="61108608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -463,7 +473,7 @@
         <c:spPr>
           <a:noFill/>
         </c:spPr>
-        <c:crossAx val="62830848"/>
+        <c:crossAx val="61012608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="20"/>
@@ -496,9 +506,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.73570822397200364"/>
-          <c:y val="0.16755043013391036"/>
-          <c:w val="0.24484733158355212"/>
-          <c:h val="0.15488984556817084"/>
+          <c:y val="0.16755043013391038"/>
+          <c:w val="0.24484733158355218"/>
+          <c:h val="0.15488984556817087"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -521,7 +531,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -650,25 +660,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="63071360"/>
-        <c:axId val="63345024"/>
+        <c:axId val="61024128"/>
+        <c:axId val="61025664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="63071360"/>
+        <c:axId val="61024128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63345024"/>
+        <c:crossAx val="61025664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63345024"/>
+        <c:axId val="61025664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -696,7 +706,7 @@
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63071360"/>
+        <c:crossAx val="61024128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="20"/>
@@ -721,8 +731,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.79650338228269379"/>
-          <c:y val="0.15320456256640852"/>
+          <c:x val="0.79650338228269368"/>
+          <c:y val="0.15320456256640858"/>
           <c:w val="0.17479472600171553"/>
           <c:h val="0.14658476001491769"/>
         </c:manualLayout>
@@ -742,7 +752,203 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="34"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sr-Latn-CS" baseline="0">
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Sorting performance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" baseline="0">
+              <a:latin typeface="+mn-lt"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sorting!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>java</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sorting!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>test #1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sorting!$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sorting!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>jodd merge</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sorting!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>test #1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sorting!$F$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>52.438384897745152</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="75"/>
+        <c:overlap val="40"/>
+        <c:axId val="62728448"/>
+        <c:axId val="62815616"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="62728448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="62815616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="62815616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sr-Latn-CS" sz="1100" baseline="0"/>
+                  <a:t>Time [%]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="62728448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="20"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.78104851207714343"/>
+          <c:y val="8.3215750846157635E-2"/>
+          <c:w val="0.19829036281001655"/>
+          <c:h val="0.14658476001491769"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -836,6 +1042,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1249,8 +1490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1303,4 +1544,56 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1907</v>
+      </c>
+      <c r="C2">
+        <v>1000</v>
+      </c>
+      <c r="D2">
+        <v>6579</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <f>C2/B2 * 100</f>
+        <v>52.438384897745152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>